<commit_message>
resubmit draft 1 and 2
</commit_message>
<xml_diff>
--- a/Misc/Phrase Contribution Chart.xlsx
+++ b/Misc/Phrase Contribution Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentvcc-my.sharepoint.com/personal/000437017_student_vcc_ca/Documents/Winter 2021/CSTP 1304 User Interface Design/Lo-farm Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CSTP1304_SuperGreenTeam\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{A37518FB-5439-49B2-84D3-8A29C2D085C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4B3FFD6A-61EE-4BF3-A691-D128A1ED1347}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9682A2-7DE8-470F-AABC-956EA3DBF0D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{94F45A5A-809A-4065-90BC-2CC3DFE7252F}"/>
   </bookViews>
@@ -119,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -130,6 +130,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0F75F8-C6F4-403D-9F5C-4BE06D7D124F}">
-  <dimension ref="A2:D6"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A3:D6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,63 +459,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:4" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>